<commit_message>
Dodan detaljniji opis scenarija
</commit_message>
<xml_diff>
--- a/UseCaseIScenarij/KreiranjeNalogaScenarij.xlsx
+++ b/UseCaseIScenarij/KreiranjeNalogaScenarij.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
   <si>
     <t>Kreiranje korisničkog računa</t>
   </si>
@@ -33,9 +33,6 @@
     <t xml:space="preserve">unošenjem osnovnih podataka. U slučaju da račun kreira doktor, </t>
   </si>
   <si>
-    <t>zahtijevaju se dodatni podaci. Admin mora potvrditi kreiranje računa doktora.</t>
-  </si>
-  <si>
     <t>Glavni tok:</t>
   </si>
   <si>
@@ -45,16 +42,10 @@
     <t>Korisnik ima dostupnu aplikaciju</t>
   </si>
   <si>
-    <t>Posljedice:</t>
-  </si>
-  <si>
     <t>Korisnički račun je uspješno kreiran, a korisnik može zakazivati preglede,</t>
   </si>
   <si>
     <t>pregledati historiju pregleda, pisati izvještaje, komentarisati...</t>
-  </si>
-  <si>
-    <t>SCENARIJ I</t>
   </si>
   <si>
     <t>Tok događaja:</t>
@@ -129,9 +120,6 @@
     <t>računa doktora</t>
   </si>
   <si>
-    <t>3. Unos ličnih podataka:</t>
-  </si>
-  <si>
     <t>2. Unos ličnih podataka</t>
   </si>
   <si>
@@ -159,7 +147,43 @@
     <t>6. Kreiranje računa</t>
   </si>
   <si>
-    <t>Korisnik unosi potrebne podatke. Završava se uspješnom registracijom korisnika</t>
+    <t>SCENARIJ BROJ 1</t>
+  </si>
+  <si>
+    <t>Vezani zahtjevi:</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>Korisnik unosi potrebne podatke o sebi</t>
+  </si>
+  <si>
+    <t>Posljedice (uspješan završetak):</t>
+  </si>
+  <si>
+    <t>Posljedice (neuspješan završetak):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Korisnički račun nije kreiran. Nemoguće je pristupiti osnovnim </t>
+  </si>
+  <si>
+    <t>Primarni akteri:</t>
+  </si>
+  <si>
+    <t>Pacijent, doktor</t>
+  </si>
+  <si>
+    <t>Ostali akteri:</t>
+  </si>
+  <si>
+    <t>zahtijevaju se dodatni podaci. Admin mora potvrditi kreiranje računa doktora</t>
+  </si>
+  <si>
+    <t>funkcionalnostima aplikacije</t>
+  </si>
+  <si>
+    <t>3. Unos ličnih podataka</t>
   </si>
 </sst>
 </file>
@@ -393,9 +417,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -406,7 +429,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -426,11 +448,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -449,34 +475,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,451 +804,542 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="A21" sqref="A21:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="17"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" s="25" customFormat="1">
+      <c r="A3" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="52"/>
+      <c r="D3" s="52"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="52"/>
+      <c r="I3" s="53"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="33"/>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="11"/>
+      <c r="B5" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="55"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
+      <c r="G5" s="55"/>
+      <c r="H5" s="55"/>
+      <c r="I5" s="64"/>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="16"/>
+      <c r="B6" s="62" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="29"/>
+      <c r="H6" s="29"/>
+      <c r="I6" s="30"/>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="B7" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="52"/>
+      <c r="D7" s="52"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="52"/>
+      <c r="H7" s="52"/>
+      <c r="I7" s="53"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="69" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="48"/>
+    </row>
+    <row r="9" spans="1:9" s="25" customFormat="1">
+      <c r="A9" s="70" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
+      <c r="I9" s="40"/>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="71"/>
+      <c r="B10" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="57"/>
+      <c r="D10" s="57"/>
+      <c r="E10" s="57"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="57"/>
+      <c r="H10" s="57"/>
+      <c r="I10" s="58"/>
+    </row>
+    <row r="11" spans="1:9" s="25" customFormat="1">
+      <c r="A11" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="72" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="73"/>
+    </row>
+    <row r="12" spans="1:9" s="25" customFormat="1">
+      <c r="A12" s="26"/>
+      <c r="B12" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="49"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="50"/>
+    </row>
+    <row r="13" spans="1:9" s="25" customFormat="1">
+      <c r="A13" s="66" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="53"/>
+    </row>
+    <row r="14" spans="1:9" s="25" customFormat="1">
+      <c r="A14" s="74" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="44" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="61"/>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="75" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="75"/>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="67"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="76" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="1:7" s="25" customFormat="1">
+      <c r="A20" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="19"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-    </row>
-    <row r="3" spans="1:9" s="27" customFormat="1">
-      <c r="A3" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="45" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="46"/>
-      <c r="E3" s="46"/>
-      <c r="F3" s="46"/>
-      <c r="G3" s="46"/>
-      <c r="H3" s="46"/>
-      <c r="I3" s="47"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="64" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="65"/>
-      <c r="D4" s="65"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="65"/>
-      <c r="H4" s="65"/>
-      <c r="I4" s="66"/>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="13"/>
-      <c r="B5" s="62" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="63"/>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="18"/>
-      <c r="B6" s="59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="61"/>
-    </row>
-    <row r="7" spans="1:9" s="27" customFormat="1">
-      <c r="A7" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="47"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="56" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="57"/>
-      <c r="D8" s="57"/>
-      <c r="E8" s="57"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
-      <c r="H8" s="57"/>
-      <c r="I8" s="58"/>
-    </row>
-    <row r="9" spans="1:9" s="27" customFormat="1">
-      <c r="A9" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="37"/>
-      <c r="H9" s="37"/>
-      <c r="I9" s="38"/>
-    </row>
-    <row r="10" spans="1:9" s="27" customFormat="1">
-      <c r="A10" s="14"/>
-      <c r="B10" s="52" t="s">
+      <c r="B20" s="52"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="32"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="19"/>
+      <c r="E21" s="19"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="B22" s="29"/>
+      <c r="C22" s="30"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+    </row>
+    <row r="23" spans="1:7" s="25" customFormat="1">
+      <c r="A23" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="7"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B24" s="32"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B25" s="29"/>
+      <c r="C25" s="30"/>
+      <c r="D25" s="16"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="54" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27" s="55"/>
+      <c r="C27" s="55"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="55"/>
+      <c r="F27" s="55"/>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="53"/>
-      <c r="D10" s="53"/>
-      <c r="E10" s="53"/>
-      <c r="F10" s="53"/>
-      <c r="G10" s="53"/>
-      <c r="H10" s="53"/>
-      <c r="I10" s="54"/>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="55"/>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="33" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14" s="34"/>
-      <c r="C14" s="35"/>
-      <c r="D14" s="16" t="s">
+      <c r="B29" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C29" s="36"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="37"/>
+      <c r="G29" s="1"/>
+    </row>
+    <row r="30" spans="1:7" s="25" customFormat="1">
+      <c r="A30" s="20"/>
+      <c r="B30" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="18"/>
+    </row>
+    <row r="31" spans="1:7" s="25" customFormat="1">
+      <c r="A31" s="12"/>
+      <c r="B31" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="16" t="s">
+      <c r="C31" s="42"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="18"/>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32" s="14"/>
+      <c r="B32" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" s="27" customFormat="1">
-      <c r="A15" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="B15" s="46"/>
-      <c r="C15" s="47"/>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="20"/>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="48" t="s">
+      <c r="C32" s="45"/>
+      <c r="D32" s="46"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="1"/>
+    </row>
+    <row r="33" spans="1:7" s="25" customFormat="1">
+      <c r="A33" s="20"/>
+      <c r="B33" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="39"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="38" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="40"/>
+      <c r="G33" s="18"/>
+    </row>
+    <row r="34" spans="1:7" s="25" customFormat="1">
+      <c r="A34" s="12"/>
+      <c r="B34" s="56" t="s">
+        <v>23</v>
+      </c>
+      <c r="C34" s="57"/>
+      <c r="D34" s="58"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="27"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="C38" s="36"/>
+      <c r="D38" s="37"/>
+      <c r="E38" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="65"/>
-      <c r="C16" s="66"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-    </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="69" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="60"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="18"/>
-      <c r="E17" s="18"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-    </row>
-    <row r="18" spans="1:7" s="27" customFormat="1">
-      <c r="A18" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="8"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="20"/>
-    </row>
-    <row r="19" spans="1:7">
-      <c r="A19" s="48" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" s="65"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-    </row>
-    <row r="20" spans="1:7">
-      <c r="A20" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="60"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="18"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-    </row>
-    <row r="22" spans="1:7">
-      <c r="A22" s="50" t="s">
+      <c r="F38" s="37"/>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="38"/>
+      <c r="C39" s="39"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="24"/>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="41"/>
+      <c r="C40" s="42"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="5"/>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="2"/>
-    </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="1:7">
-      <c r="A24" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B24" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="F24" s="35"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="1:7" s="27" customFormat="1">
-      <c r="A25" s="22"/>
-      <c r="B25" s="36" t="s">
-        <v>22</v>
-      </c>
-      <c r="C25" s="37"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="25"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="20"/>
-    </row>
-    <row r="26" spans="1:7" s="27" customFormat="1">
-      <c r="A26" s="14"/>
-      <c r="B26" s="39" t="s">
-        <v>23</v>
-      </c>
-      <c r="C26" s="40"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="20"/>
-    </row>
-    <row r="27" spans="1:7">
-      <c r="A27" s="16"/>
-      <c r="B27" s="42" t="s">
-        <v>25</v>
-      </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="44"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="2"/>
-    </row>
-    <row r="28" spans="1:7" s="27" customFormat="1">
-      <c r="A28" s="28"/>
-      <c r="B28" s="48" t="s">
-        <v>26</v>
-      </c>
-      <c r="C28" s="70"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="48" t="s">
-        <v>28</v>
-      </c>
-      <c r="F28" s="49"/>
-      <c r="G28" s="20"/>
-    </row>
-    <row r="29" spans="1:7" s="27" customFormat="1">
-      <c r="A29" s="29"/>
-      <c r="B29" s="68" t="s">
-        <v>27</v>
-      </c>
-      <c r="C29" s="71"/>
-      <c r="D29" s="72"/>
-      <c r="E29" s="30"/>
-      <c r="F29" s="31"/>
-    </row>
-    <row r="31" spans="1:7">
-      <c r="A31" s="67" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-    </row>
-    <row r="33" spans="1:6">
-      <c r="A33" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="B33" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" s="34"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="33" t="s">
-        <v>21</v>
-      </c>
-      <c r="F33" s="35"/>
-    </row>
-    <row r="34" spans="1:6">
-      <c r="A34" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="B34" s="36"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="26"/>
-    </row>
-    <row r="35" spans="1:6">
-      <c r="A35" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="B35" s="39"/>
-      <c r="C35" s="40"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="6"/>
-    </row>
-    <row r="36" spans="1:6">
-      <c r="A36" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="10"/>
-      <c r="F36" s="7"/>
-    </row>
-    <row r="37" spans="1:6" s="27" customFormat="1">
-      <c r="A37" s="20"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="32"/>
-      <c r="E37" s="32"/>
-      <c r="F37" s="32"/>
-    </row>
-    <row r="38" spans="1:6" s="27" customFormat="1">
-      <c r="A38" s="20"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="46"/>
+      <c r="E41" s="9"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:7" s="25" customFormat="1">
+      <c r="A42" s="18"/>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42" s="59"/>
+      <c r="F42" s="59"/>
+    </row>
+    <row r="43" spans="1:7" s="25" customFormat="1">
+      <c r="A43" s="18"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
+      <c r="E43" s="18"/>
+      <c r="F43" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="33">
-    <mergeCell ref="A31:G31"/>
+  <mergeCells count="38">
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="A17:E17"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="E42:F42"/>
+    <mergeCell ref="B3:I3"/>
+    <mergeCell ref="B9:I9"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="A27:F27"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="A19:C19"/>
     <mergeCell ref="A20:C20"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A16:C16"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="B3:I3"/>
-    <mergeCell ref="B7:I7"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="B9:I9"/>
     <mergeCell ref="B10:I10"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B8:I8"/>
     <mergeCell ref="B6:I6"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="B4:I4"/>
-    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="A36:G36"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A24:C24"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
     <mergeCell ref="B33:D33"/>
-    <mergeCell ref="E33:F33"/>
     <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="E37:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>